<commit_message>
Added selendroid fix for scroll
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Tabbar_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Tabbar_JS.xlsx
@@ -344,6 +344,110 @@
 </t>
   </si>
   <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Native Tabbar JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0576
+};
+validate4
+{
+validate_Screenshot=VT200_0578_before
+};
+validate5
+{
+validate_Text_Exists=VT200-0578
+};
+validate6
+{
+validate_Screenshot=VT200_0578
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Native Tabbar JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0576
+};
+validate4
+{
+validate_Screenshot=VT200_0595_before
+};
+validate5
+{
+validate_Text_Exists=VT200-0595
+};
+validate6
+{
+validate_Screenshot=VT200_0595
+};
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Native Tabbar JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0576
+};
+validate4
+{
+validate_Screenshot=VT200_0596_before
+};
+validate5
+{
+validate_Text_Exists=VT200-0596
+};
+validate6
+{
+validate_Screenshot=VT200_0596
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Native Tabbar JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0585
+};
+validate4
+{
+validate_Screenshot=VT200_0585
+};</t>
+  </si>
+  <si>
+    <t>Change Start page</t>
+  </si>
+  <si>
+    <t>wait(3);
+SetStartPage(http://127.0.0.1:8082/app/);</t>
+  </si>
+  <si>
     <t>wait(5);
 validate1;
 link_Click(tabbar_test_link);
@@ -357,7 +461,7 @@
 validate4;
 SwitchApp(NATIVE_APP);
 wait(2);
-link_Click(VT200_0576_mainpage_xpath);
+ClickNativeIcon(VT200_0576_mainpage_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 SelectTestToRun(VT200_0578_string);
@@ -367,32 +471,6 @@
 wait(5);
 TakeNativeScreenshot(VT200_0578);
 validate6;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Native Tabbar JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0576
-};
-validate4
-{
-validate_Screenshot=VT200_0578_before
-};
-validate5
-{
-validate_Text_Exists=VT200-0578
-};
-validate6
-{
-validate_Screenshot=VT200_0578
-};</t>
   </si>
   <si>
     <t xml:space="preserve">wait(5);
@@ -408,7 +486,7 @@
 validate4;
 SwitchApp(NATIVE_APP);
 wait(2);
-link_Click(VT200_0576_mainpage_xpath);
+ClickNativeIcon(VT200_0576_mainpage_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 SelectTestToRun(VT200_0595_string);
@@ -418,33 +496,6 @@
 wait(5);
 TakeNativeScreenshot(VT200_0595);
 validate6;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Native Tabbar JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0576
-};
-validate4
-{
-validate_Screenshot=VT200_0595_before
-};
-validate5
-{
-validate_Text_Exists=VT200-0595
-};
-validate6
-{
-validate_Screenshot=VT200_0595
-};
 </t>
   </si>
   <si>
@@ -461,7 +512,7 @@
 validate4;
 SwitchApp(NATIVE_APP);
 wait(2);
-link_Click(VT200_0576_mainpage_xpath);
+ClickNativeIcon(VT200_0576_mainpage_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 SelectTestToRun(VT200_0596_string);
@@ -471,50 +522,6 @@
 wait(5);
 TakeNativeScreenshot(VT200_0596);
 validate6;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Native Tabbar JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0576
-};
-validate4
-{
-validate_Screenshot=VT200_0596_before
-};
-validate5
-{
-validate_Text_Exists=VT200-0596
-};
-validate6
-{
-validate_Screenshot=VT200_0596
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Native Tabbar JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0585
-};
-validate4
-{
-validate_Screenshot=VT200_0585
-};</t>
   </si>
   <si>
     <t>wait(5);
@@ -530,15 +537,8 @@
 validate4;
 SwitchApp(NATIVE_APP);
 wait(2);
-link_Click(VT200_0585_page1_xpath);
+ClickNativeIcon(VT200_0585_page1_xpath);
 CheckUITextContains(1);</t>
-  </si>
-  <si>
-    <t>Change Start page</t>
-  </si>
-  <si>
-    <t>wait(3);
-SetStartPage(http://127.0.0.1:8082/app/);</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1030,13 +1030,13 @@
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="2" t="s">
@@ -1117,10 +1117,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1171,10 +1171,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1198,10 +1198,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1306,10 +1306,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>

</xml_diff>